<commit_message>
- [DOC_02] Changement du tag de navigation pour les news ("RH"). Une news ne peut pas être tagguée avec "news" mais avec une sosu catégorie. - Ajustement des Display Templates pour n'utiliser que des propriétés existantes sur les éléments de catalogues. Si les propriétés ne sont pas en concordance avec le result type (DisplayProperties dans ResultTypeInfo) alors cela provoque une erreur d'affichage au moment de la recherche.
</commit_message>
<xml_diff>
--- a/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/NewsPages.xlsx
+++ b/Source/GSoft.Dynamite.CrossSitePublishingCMS/Modules/Docs/DOC_02/Default/NewsPages.xlsx
@@ -85,9 +85,6 @@
 Curabitur ullamcorper ultricies nisi.</t>
   </si>
   <si>
-    <t>News</t>
-  </si>
-  <si>
     <t>Approved</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>DynamiteImageDescription</t>
+  </si>
+  <si>
+    <t>HR</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,40 +549,40 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -609,10 +609,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>7</v>
@@ -630,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q2"/>
       <c r="R2"/>

</xml_diff>